<commit_message>
prep_server success 媛쒖꽑, app.py ?ㅽ? ?섏젙, .gitignore??success-preview ?쒖쇅
- success.html: stage-panel 1030px, Paperlogy CDN, header-bar 475x150, TIE ?붾? ?곗씠??- app.py: datetime import ?ㅽ? ?쒓굅
- .gitignore: success-preview.html ?꾩떆?뚯씪 ?쒖쇅
- admin, assets, backend, register ???섏젙?ы빆 諛섏쁺
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fktl3\OneDrive\바탕 화면\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minmi\Documents\00-html-play\project-root\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72D2CF57-799C-4840-890F-2945E9EA409D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9CA712-A851-44E7-B86C-A7FDB9DD53ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49530" yWindow="4030" windowWidth="29300" windowHeight="16830" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="765" windowWidth="28470" windowHeight="13725" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -480,14 +480,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>LODON LIBERTY TOILE · SIZE S · BLACK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LODON LIBERTY TOILE · SIZE L · BLACK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>SOLID SUIT SLIM TIE · BLACK</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -496,10 +488,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>SOLID SUIT SKINNY TIE · GREY</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>TENEU SOLID · SIZE S · LIGHT BLUE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -592,6 +580,18 @@
   </si>
   <si>
     <t>TENEU SOLID PINTUCK · SIZE M · WHITE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONDON LIBERTY TOILE · SIZE S · BLACK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONDON LIBERTY TOILE · SIZE L · BLACK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOLID SUIT SLIM TIE · GREY</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -943,20 +943,20 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -973,10 +973,10 @@
         <v>115</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -990,13 +990,13 @@
         <v>106</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1010,13 +1010,13 @@
         <v>106</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1030,13 +1030,13 @@
         <v>106</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1050,13 +1050,13 @@
         <v>106</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1070,13 +1070,13 @@
         <v>106</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1090,13 +1090,13 @@
         <v>106</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1110,13 +1110,13 @@
         <v>107</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1130,13 +1130,13 @@
         <v>107</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1153,10 +1153,10 @@
         <v>116</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1173,10 +1173,10 @@
         <v>116</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1193,10 +1193,10 @@
         <v>117</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1213,94 +1213,94 @@
         <v>117</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>52</v>
       </c>
@@ -1314,14 +1314,14 @@
         <v>108</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
@@ -1335,14 +1335,14 @@
         <v>108</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
@@ -1356,14 +1356,14 @@
         <v>108</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -1377,14 +1377,14 @@
         <v>108</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>57</v>
       </c>
@@ -1401,11 +1401,11 @@
         <v>120</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>56</v>
       </c>
@@ -1422,11 +1422,11 @@
         <v>120</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>58</v>
       </c>
@@ -1443,11 +1443,11 @@
         <v>121</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>59</v>
       </c>
@@ -1464,11 +1464,11 @@
         <v>121</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>60</v>
       </c>
@@ -1485,10 +1485,10 @@
         <v>118</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>61</v>
       </c>
@@ -1505,10 +1505,10 @@
         <v>118</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>62</v>
       </c>
@@ -1525,10 +1525,10 @@
         <v>119</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>63</v>
       </c>
@@ -1545,10 +1545,10 @@
         <v>119</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>64</v>
       </c>
@@ -1565,10 +1565,10 @@
         <v>122</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>65</v>
       </c>
@@ -1585,11 +1585,11 @@
         <v>122</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>85</v>
       </c>
@@ -1606,11 +1606,11 @@
         <v>123</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>86</v>
       </c>
@@ -1627,11 +1627,11 @@
         <v>123</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -1645,14 +1645,14 @@
         <v>112</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>67</v>
       </c>
@@ -1666,14 +1666,14 @@
         <v>112</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>68</v>
       </c>
@@ -1687,14 +1687,14 @@
         <v>112</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>69</v>
       </c>
@@ -1708,14 +1708,14 @@
         <v>112</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>75</v>
       </c>
@@ -1729,13 +1729,13 @@
         <v>114</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
@@ -1749,13 +1749,13 @@
         <v>114</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>71</v>
       </c>
@@ -1769,13 +1769,13 @@
         <v>113</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>72</v>
       </c>
@@ -1789,13 +1789,13 @@
         <v>113</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>73</v>
       </c>
@@ -1809,13 +1809,13 @@
         <v>113</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>74</v>
       </c>
@@ -1829,10 +1829,10 @@
         <v>113</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>